<commit_message>
Inclusão do Gustavo, colocação das colunas do dataset em tabelas.
</commit_message>
<xml_diff>
--- a/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
+++ b/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B3D45E-3A71-49BB-AC09-65CBFAFC50EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958DD7D9-152C-4EC8-85FA-2A60B9105B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25810" yWindow="4780" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="ColumnTitle1">'Controlador de projetos'!$B$4</definedName>
     <definedName name="ColumnTitle2">Tabela_de_categorias_e_funcionários[[#Headers],[Nome da Categoria]]</definedName>
     <definedName name="Funcionário_Lista">Configuração!$D$5:$D$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$L$13</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Controlador de projetos'!$4:$4</definedName>
     <definedName name="Sinalizador_Porcentagem">'Controlador de projetos'!#REF!</definedName>
   </definedNames>
@@ -1382,7 +1383,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" sqref="A1:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -2108,7 +2109,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Reorganização de pastas, cronograma e glossário
</commit_message>
<xml_diff>
--- a/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
+++ b/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4562463B-9BA7-40A4-B14C-927B904CCE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D85E691-D3EC-4645-AC43-2DE99BD9F71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25810" yWindow="4780" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24460" yWindow="5640" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controlador de projetos" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
   <si>
     <t>Categoria</t>
   </si>
@@ -164,6 +164,33 @@
   </si>
   <si>
     <t>População do Sumário</t>
+  </si>
+  <si>
+    <t>Proposta Anaíltca</t>
+  </si>
+  <si>
+    <t>Análise Exploratória</t>
+  </si>
+  <si>
+    <t>Scripts Análise Exploratória</t>
+  </si>
+  <si>
+    <t>Esboço Sotory Telling</t>
+  </si>
+  <si>
+    <t>Revisão Scripts A.E.</t>
+  </si>
+  <si>
+    <t>A. E. no relatório</t>
+  </si>
+  <si>
+    <t>Video Story Telling</t>
+  </si>
+  <si>
+    <t>Relatório Final</t>
+  </si>
+  <si>
+    <t>Atualizado em 2025-03-07</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1416,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -1414,7 +1441,9 @@
     <row r="2" spans="1:12" ht="20.25" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="D2" s="6"/>
       <c r="E2" s="3"/>
     </row>
@@ -1795,23 +1824,37 @@
       <c r="I14" s="14">
         <v>45719</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="15" t="str">
+      <c r="J14" s="13">
+        <v>45723</v>
+      </c>
+      <c r="K14" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I14,'Controlador de projetos'!$J14)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I14,'Controlador de projetos'!$J14,FALSE)+1)</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="L14" s="12"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="19" t="str">
+      <c r="B15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="13">
+        <v>45719</v>
+      </c>
+      <c r="G15" s="13">
+        <v>45741</v>
+      </c>
+      <c r="H15" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F15,'Controlador de projetos'!$G15)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F15,'Controlador de projetos'!$G15,FALSE)+1)</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="13"/>
@@ -1822,15 +1865,27 @@
       <c r="L15" s="12"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="19" t="str">
+      <c r="B16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="13">
+        <v>45719</v>
+      </c>
+      <c r="G16" s="13">
+        <v>45741</v>
+      </c>
+      <c r="H16" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F16,'Controlador de projetos'!$G16)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F16,'Controlador de projetos'!$G16,FALSE)+1)</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="13"/>
@@ -1841,15 +1896,27 @@
       <c r="L16" s="12"/>
     </row>
     <row r="17" spans="2:12" ht="30" customHeight="1">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="19" t="str">
+      <c r="B17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="13">
+        <v>45719</v>
+      </c>
+      <c r="G17" s="13">
+        <v>45741</v>
+      </c>
+      <c r="H17" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F17,'Controlador de projetos'!$G17)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F17,'Controlador de projetos'!$G17,FALSE)+1)</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="13"/>
@@ -1860,15 +1927,27 @@
       <c r="L17" s="12"/>
     </row>
     <row r="18" spans="2:12" ht="30" customHeight="1">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="19" t="str">
+      <c r="B18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="13">
+        <v>45747</v>
+      </c>
+      <c r="G18" s="13">
+        <v>45772</v>
+      </c>
+      <c r="H18" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F18,'Controlador de projetos'!$G18)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F18,'Controlador de projetos'!$G18,FALSE)+1)</f>
-        <v/>
+        <v>26</v>
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="13"/>
@@ -1879,15 +1958,27 @@
       <c r="L18" s="12"/>
     </row>
     <row r="19" spans="2:12" ht="30" customHeight="1">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="19" t="str">
+      <c r="B19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="13">
+        <v>45747</v>
+      </c>
+      <c r="G19" s="13">
+        <v>45772</v>
+      </c>
+      <c r="H19" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F19,'Controlador de projetos'!$G19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F19,'Controlador de projetos'!$G19,FALSE)+1)</f>
-        <v/>
+        <v>26</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="13"/>
@@ -1898,15 +1989,27 @@
       <c r="L19" s="12"/>
     </row>
     <row r="20" spans="2:12" ht="30" customHeight="1">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="19" t="str">
+      <c r="B20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="13">
+        <v>45747</v>
+      </c>
+      <c r="G20" s="13">
+        <v>45772</v>
+      </c>
+      <c r="H20" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F20,'Controlador de projetos'!$G20)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F20,'Controlador de projetos'!$G20,FALSE)+1)</f>
-        <v/>
+        <v>26</v>
       </c>
       <c r="I20" s="14"/>
       <c r="J20" s="13"/>
@@ -1917,15 +2020,27 @@
       <c r="L20" s="12"/>
     </row>
     <row r="21" spans="2:12" ht="30" customHeight="1">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="19" t="str">
+      <c r="B21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="13">
+        <v>45775</v>
+      </c>
+      <c r="G21" s="13">
+        <v>45800</v>
+      </c>
+      <c r="H21" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F21,'Controlador de projetos'!$G21)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F21,'Controlador de projetos'!$G21,FALSE)+1)</f>
-        <v/>
+        <v>26</v>
       </c>
       <c r="I21" s="14"/>
       <c r="J21" s="13"/>
@@ -1936,15 +2051,27 @@
       <c r="L21" s="12"/>
     </row>
     <row r="22" spans="2:12" ht="30" customHeight="1">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="19" t="str">
+      <c r="B22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="13">
+        <v>45775</v>
+      </c>
+      <c r="G22" s="13">
+        <v>45800</v>
+      </c>
+      <c r="H22" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F22,'Controlador de projetos'!$G22)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F22,'Controlador de projetos'!$G22,FALSE)+1)</f>
-        <v/>
+        <v>26</v>
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="13"/>

</xml_diff>

<commit_message>
Pastas novas para AE fase 2
</commit_message>
<xml_diff>
--- a/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
+++ b/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D85E691-D3EC-4645-AC43-2DE99BD9F71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1792F0B-94A9-4FAE-8AB4-DA55E6597837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24460" yWindow="5640" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="ColumnTitle1">'Controlador de projetos'!$B$4</definedName>
     <definedName name="ColumnTitle2">Tabela_de_categorias_e_funcionários[[#Headers],[Nome da Categoria]]</definedName>
     <definedName name="Funcionário_Lista">Configuração!$D$5:$D$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$L$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$L$30</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Controlador de projetos'!$4:$4</definedName>
     <definedName name="Sinalizador_Porcentagem">'Controlador de projetos'!#REF!</definedName>
   </definedNames>
@@ -1416,7 +1416,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" sqref="A1:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -2256,7 +2256,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Atualização do Cronograma para fase 2
</commit_message>
<xml_diff>
--- a/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
+++ b/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1792F0B-94A9-4FAE-8AB4-DA55E6597837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8FD702-4555-411B-8C9E-EB473CB164EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24460" yWindow="5640" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25120" yWindow="4950" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controlador de projetos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="ColumnTitle1">'Controlador de projetos'!$B$4</definedName>
     <definedName name="ColumnTitle2">Tabela_de_categorias_e_funcionários[[#Headers],[Nome da Categoria]]</definedName>
     <definedName name="Funcionário_Lista">Configuração!$D$5:$D$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$L$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$L$32</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Controlador de projetos'!$4:$4</definedName>
     <definedName name="Sinalizador_Porcentagem">'Controlador de projetos'!#REF!</definedName>
   </definedNames>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="50">
   <si>
     <t>Categoria</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>Atualizado em 2025-03-07</t>
+  </si>
+  <si>
+    <t>Revisão de Seção Objetivos</t>
+  </si>
+  <si>
+    <t>Revisão de Organização do Documento - Conforme comentário Fase 1</t>
   </si>
 </sst>
 </file>
@@ -783,7 +789,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -849,6 +855,12 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="13" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="13" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1136,8 +1148,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ControladorDeProjetos" displayName="ControladorDeProjetos" ref="B4:L30" totalsRowShown="0" tableBorderDxfId="2">
-  <autoFilter ref="B4:L30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ControladorDeProjetos" displayName="ControladorDeProjetos" ref="B4:L32" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="B4:L32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa" dataCellStyle="Texto"/>
     <tableColumn id="3" xr3:uid="{B833AB72-8646-4CE5-98B8-9D4D27103F03}" name="Responsável" dataCellStyle="Texto"/>
@@ -1412,11 +1424,11 @@
     <tabColor theme="9"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L30"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -1812,14 +1824,14 @@
         <v>10</v>
       </c>
       <c r="F14" s="13">
-        <v>45719</v>
+        <v>45732</v>
       </c>
       <c r="G14" s="13">
         <v>45723</v>
       </c>
       <c r="H14" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F14,'Controlador de projetos'!$G14)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F14,'Controlador de projetos'!$G14,FALSE)+1)</f>
-        <v>5</v>
+        <v>-8</v>
       </c>
       <c r="I14" s="14">
         <v>45719</v>
@@ -1847,16 +1859,18 @@
         <v>10</v>
       </c>
       <c r="F15" s="13">
-        <v>45719</v>
+        <v>45732</v>
       </c>
       <c r="G15" s="13">
         <v>45741</v>
       </c>
       <c r="H15" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F15,'Controlador de projetos'!$G15)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F15,'Controlador de projetos'!$G15,FALSE)+1)</f>
-        <v>23</v>
-      </c>
-      <c r="I15" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="I15" s="14">
+        <v>45740</v>
+      </c>
       <c r="J15" s="13"/>
       <c r="K15" s="15" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$I15,'Controlador de projetos'!$J15)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I15,'Controlador de projetos'!$J15,FALSE)+1)</f>
@@ -1878,16 +1892,18 @@
         <v>21</v>
       </c>
       <c r="F16" s="13">
-        <v>45719</v>
+        <v>45732</v>
       </c>
       <c r="G16" s="13">
-        <v>45741</v>
+        <v>45740</v>
       </c>
       <c r="H16" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F16,'Controlador de projetos'!$G16)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F16,'Controlador de projetos'!$G16,FALSE)+1)</f>
-        <v>23</v>
-      </c>
-      <c r="I16" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="I16" s="14">
+        <v>45740</v>
+      </c>
       <c r="J16" s="13"/>
       <c r="K16" s="15" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$I16,'Controlador de projetos'!$J16)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I16,'Controlador de projetos'!$J16,FALSE)+1)</f>
@@ -1909,16 +1925,18 @@
         <v>12</v>
       </c>
       <c r="F17" s="13">
-        <v>45719</v>
+        <v>45732</v>
       </c>
       <c r="G17" s="13">
-        <v>45741</v>
+        <v>45740</v>
       </c>
       <c r="H17" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F17,'Controlador de projetos'!$G17)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F17,'Controlador de projetos'!$G17,FALSE)+1)</f>
-        <v>23</v>
-      </c>
-      <c r="I17" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="I17" s="14">
+        <v>45733</v>
+      </c>
       <c r="J17" s="13"/>
       <c r="K17" s="15" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$I17,'Controlador de projetos'!$J17)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I17,'Controlador de projetos'!$J17,FALSE)+1)</f>
@@ -1928,69 +1946,71 @@
     </row>
     <row r="18" spans="2:12" ht="30" customHeight="1">
       <c r="B18" s="12" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F18" s="13">
-        <v>45747</v>
+        <v>45732</v>
       </c>
       <c r="G18" s="13">
-        <v>45772</v>
+        <v>45740</v>
       </c>
       <c r="H18" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F18,'Controlador de projetos'!$G18)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F18,'Controlador de projetos'!$G18,FALSE)+1)</f>
-        <v>26</v>
-      </c>
-      <c r="I18" s="14"/>
+        <f>IF(COUNTA('Controlador de projetos'!$F18,'Controlador de projetos'!$G18)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F18,'Controlador de projetos'!$G18,FALSE))</f>
+        <v>8</v>
+      </c>
+      <c r="I18" s="22">
+        <v>45733</v>
+      </c>
       <c r="J18" s="13"/>
       <c r="K18" s="15" t="str">
-        <f>IF(COUNTA('Controlador de projetos'!$I18,'Controlador de projetos'!$J18)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I18,'Controlador de projetos'!$J18,FALSE)+1)</f>
-        <v/>
-      </c>
-      <c r="L18" s="12"/>
-    </row>
-    <row r="19" spans="2:12" ht="30" customHeight="1">
+        <f>IF(COUNTA('Controlador de projetos'!$I18,'Controlador de projetos'!$J18)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I18,'Controlador de projetos'!$J18,FALSE))</f>
+        <v/>
+      </c>
+      <c r="L18" s="23"/>
+    </row>
+    <row r="19" spans="2:12" ht="42.5" customHeight="1">
       <c r="B19" s="12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F19" s="13">
+        <v>45742</v>
+      </c>
+      <c r="G19" s="13">
         <v>45747</v>
       </c>
-      <c r="G19" s="13">
-        <v>45772</v>
-      </c>
       <c r="H19" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F19,'Controlador de projetos'!$G19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F19,'Controlador de projetos'!$G19,FALSE)+1)</f>
-        <v>26</v>
-      </c>
-      <c r="I19" s="14"/>
+        <f>IF(COUNTA('Controlador de projetos'!$F19,'Controlador de projetos'!$G19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F19,'Controlador de projetos'!$G19,FALSE))</f>
+        <v>5</v>
+      </c>
+      <c r="I19" s="22"/>
       <c r="J19" s="13"/>
       <c r="K19" s="15" t="str">
-        <f>IF(COUNTA('Controlador de projetos'!$I19,'Controlador de projetos'!$J19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I19,'Controlador de projetos'!$J19,FALSE)+1)</f>
-        <v/>
-      </c>
-      <c r="L19" s="12"/>
+        <f>IF(COUNTA('Controlador de projetos'!$I19,'Controlador de projetos'!$J19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I19,'Controlador de projetos'!$J19,FALSE))</f>
+        <v/>
+      </c>
+      <c r="L19" s="23"/>
     </row>
     <row r="20" spans="2:12" ht="30" customHeight="1">
       <c r="B20" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>36</v>
@@ -1999,7 +2019,7 @@
         <v>19</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F20" s="13">
         <v>45747</v>
@@ -2021,22 +2041,22 @@
     </row>
     <row r="21" spans="2:12" ht="30" customHeight="1">
       <c r="B21" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" s="13">
-        <v>45775</v>
+        <v>45747</v>
       </c>
       <c r="G21" s="13">
-        <v>45800</v>
+        <v>45772</v>
       </c>
       <c r="H21" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F21,'Controlador de projetos'!$G21)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F21,'Controlador de projetos'!$G21,FALSE)+1)</f>
@@ -2052,22 +2072,22 @@
     </row>
     <row r="22" spans="2:12" ht="30" customHeight="1">
       <c r="B22" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F22" s="13">
-        <v>45775</v>
+        <v>45747</v>
       </c>
       <c r="G22" s="13">
-        <v>45800</v>
+        <v>45772</v>
       </c>
       <c r="H22" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F22,'Controlador de projetos'!$G22)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F22,'Controlador de projetos'!$G22,FALSE)+1)</f>
@@ -2082,15 +2102,27 @@
       <c r="L22" s="12"/>
     </row>
     <row r="23" spans="2:12" ht="30" customHeight="1">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="19" t="str">
+      <c r="B23" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="13">
+        <v>45775</v>
+      </c>
+      <c r="G23" s="13">
+        <v>45800</v>
+      </c>
+      <c r="H23" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F23,'Controlador de projetos'!$G23)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F23,'Controlador de projetos'!$G23,FALSE)+1)</f>
-        <v/>
+        <v>26</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="13"/>
@@ -2101,15 +2133,27 @@
       <c r="L23" s="12"/>
     </row>
     <row r="24" spans="2:12" ht="30" customHeight="1">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="19" t="str">
+      <c r="B24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="13">
+        <v>45775</v>
+      </c>
+      <c r="G24" s="13">
+        <v>45800</v>
+      </c>
+      <c r="H24" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F24,'Controlador de projetos'!$G24)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F24,'Controlador de projetos'!$G24,FALSE)+1)</f>
-        <v/>
+        <v>26</v>
       </c>
       <c r="I24" s="14"/>
       <c r="J24" s="13"/>
@@ -2215,33 +2259,71 @@
       <c r="L29" s="12"/>
     </row>
     <row r="30" spans="2:12" ht="30" customHeight="1">
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" s="19" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$F30,'Controlador de projetos'!$G30)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F30,'Controlador de projetos'!$G30,FALSE)+1)</f>
         <v/>
       </c>
       <c r="I30" s="14"/>
-      <c r="J30" s="17"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="15" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$I30,'Controlador de projetos'!$J30)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I30,'Controlador de projetos'!$J30,FALSE)+1)</f>
         <v/>
       </c>
-      <c r="L30" s="16"/>
+      <c r="L30" s="12"/>
+    </row>
+    <row r="31" spans="2:12" ht="30" customHeight="1">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="19" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$F31,'Controlador de projetos'!$G31)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F31,'Controlador de projetos'!$G31,FALSE)+1)</f>
+        <v/>
+      </c>
+      <c r="I31" s="14"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="15" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$I31,'Controlador de projetos'!$J31)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I31,'Controlador de projetos'!$J31,FALSE)+1)</f>
+        <v/>
+      </c>
+      <c r="L31" s="12"/>
+    </row>
+    <row r="32" spans="2:12" ht="30" customHeight="1">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="19" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$F32,'Controlador de projetos'!$G32)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F32,'Controlador de projetos'!$G32,FALSE)+1)</f>
+        <v/>
+      </c>
+      <c r="I32" s="14"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="15" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$I32,'Controlador de projetos'!$J32)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I32,'Controlador de projetos'!$J32,FALSE)+1)</f>
+        <v/>
+      </c>
+      <c r="L32" s="16"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K5:K30">
+  <conditionalFormatting sqref="K5:K32">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>(ABS((K5-H5))/H5)&gt;Sinalizador_Porcentagem</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" prompt="Insira projetos nesta planilha do controle de projetos. Defina a % acima/abaixo para sinalizar em D2. O trabalho real em horas e a duração real em dias destacarão valores acima/abaixo com negrito, fonte vermelha e um ícone de bandeira nas colunas K e M " sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione uma categoria na lista ou crie uma nova categoria para exibir nesta lista da planilha Configuração." sqref="E5:E30" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione uma categoria na lista ou crie uma nova categoria para exibir nesta lista da planilha Configuração." sqref="E5:E32" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Categoria_Lista</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira os nomes de projetos nesta coluna" sqref="B4:D4" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
@@ -2271,13 +2353,13 @@
           <x14:formula1>
             <xm:f>Configuração!$D$5:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D30</xm:sqref>
+          <xm:sqref>D5:D32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9316C738-7C0B-41CA-ADB5-1A14C6ABE9FF}">
           <x14:formula1>
             <xm:f>Configuração!$C$5:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C30</xm:sqref>
+          <xm:sqref>C5:C32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Atualização do documento e cronograma.
</commit_message>
<xml_diff>
--- a/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
+++ b/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8FD702-4555-411B-8C9E-EB473CB164EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC63459D-CAD1-4561-BA15-83FAFBC23880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25120" yWindow="4950" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -789,7 +789,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -855,12 +855,6 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="13" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="13" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1428,7 +1422,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -1967,15 +1961,17 @@
         <f>IF(COUNTA('Controlador de projetos'!$F18,'Controlador de projetos'!$G18)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F18,'Controlador de projetos'!$G18,FALSE))</f>
         <v>8</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="14">
         <v>45733</v>
       </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="15" t="str">
+      <c r="J18" s="13">
+        <v>45735</v>
+      </c>
+      <c r="K18" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I18,'Controlador de projetos'!$J18)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I18,'Controlador de projetos'!$J18,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L18" s="23"/>
+        <v>2</v>
+      </c>
+      <c r="L18" s="12"/>
     </row>
     <row r="19" spans="2:12" ht="42.5" customHeight="1">
       <c r="B19" s="12" t="s">
@@ -1991,22 +1987,26 @@
         <v>10</v>
       </c>
       <c r="F19" s="13">
-        <v>45742</v>
+        <v>45732</v>
       </c>
       <c r="G19" s="13">
-        <v>45747</v>
+        <v>45740</v>
       </c>
       <c r="H19" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F19,'Controlador de projetos'!$G19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F19,'Controlador de projetos'!$G19,FALSE))</f>
-        <v>5</v>
-      </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="15" t="str">
+        <v>8</v>
+      </c>
+      <c r="I19" s="14">
+        <v>45737</v>
+      </c>
+      <c r="J19" s="13">
+        <v>45739</v>
+      </c>
+      <c r="K19" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I19,'Controlador de projetos'!$J19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I19,'Controlador de projetos'!$J19,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L19" s="23"/>
+        <v>2</v>
+      </c>
+      <c r="L19" s="12"/>
     </row>
     <row r="20" spans="2:12" ht="30" customHeight="1">
       <c r="B20" s="12" t="s">

</xml_diff>

<commit_message>
Documento Candidato a Entrega 2
</commit_message>
<xml_diff>
--- a/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
+++ b/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BF2C25-01C2-4D24-BA92-263DAFF1BB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C15AE6E-BCA6-4D28-920B-096678F0312B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="5630" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24620" yWindow="4840" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controlador de projetos" sheetId="1" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>Relatório Final</t>
   </si>
   <si>
-    <t>Atualizado em 2025-03-07</t>
-  </si>
-  <si>
     <t>Revisão de Seção Objetivos</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>Produção de gráficos e tabelas</t>
+  </si>
+  <si>
+    <t>Atualizado em 2025-04-02</t>
   </si>
 </sst>
 </file>
@@ -801,7 +801,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -867,12 +867,6 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="13" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="13" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1440,7 +1434,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -1466,7 +1460,7 @@
       <c r="A2" s="2"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="3"/>
@@ -1883,10 +1877,12 @@
       <c r="I15" s="14">
         <v>45740</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="15" t="str">
+      <c r="J15" s="13">
+        <v>45749</v>
+      </c>
+      <c r="K15" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I15,'Controlador de projetos'!$J15)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I15,'Controlador de projetos'!$J15,FALSE)+1)</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="L15" s="12"/>
     </row>
@@ -1916,10 +1912,12 @@
       <c r="I16" s="14">
         <v>45740</v>
       </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="15" t="str">
+      <c r="J16" s="13">
+        <v>45744</v>
+      </c>
+      <c r="K16" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I16,'Controlador de projetos'!$J16)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I16,'Controlador de projetos'!$J16,FALSE)+1)</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="L16" s="12"/>
     </row>
@@ -1949,16 +1947,18 @@
       <c r="I17" s="14">
         <v>45733</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="15" t="str">
+      <c r="J17" s="13">
+        <v>45744</v>
+      </c>
+      <c r="K17" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I17,'Controlador de projetos'!$J17)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I17,'Controlador de projetos'!$J17,FALSE)+1)</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="L17" s="12"/>
     </row>
     <row r="18" spans="2:12" ht="30" customHeight="1">
       <c r="B18" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>37</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="19" spans="2:12" ht="30" customHeight="1">
       <c r="B19" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>35</v>
@@ -2014,19 +2014,21 @@
         <f>IF(COUNTA('Controlador de projetos'!$F19,'Controlador de projetos'!$G19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F19,'Controlador de projetos'!$G19,FALSE))</f>
         <v>12</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="14">
         <v>45736</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="15" t="str">
+      <c r="J19" s="13">
+        <v>45739</v>
+      </c>
+      <c r="K19" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I19,'Controlador de projetos'!$J19)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I19,'Controlador de projetos'!$J19,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L19" s="23"/>
+        <v>3</v>
+      </c>
+      <c r="L19" s="12"/>
     </row>
     <row r="20" spans="2:12" ht="30" customHeight="1">
       <c r="B20" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>32</v>
@@ -2037,7 +2039,7 @@
       <c r="E20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="14">
         <v>45742</v>
       </c>
       <c r="G20" s="13">
@@ -2047,19 +2049,21 @@
         <f>IF(COUNTA('Controlador de projetos'!$F20,'Controlador de projetos'!$G20)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F20,'Controlador de projetos'!$G20,FALSE))</f>
         <v>2</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="14">
         <v>45742</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="15" t="str">
+      <c r="J20" s="13">
+        <v>45744</v>
+      </c>
+      <c r="K20" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I20,'Controlador de projetos'!$J20)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I20,'Controlador de projetos'!$J20,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L20" s="23"/>
+        <v>2</v>
+      </c>
+      <c r="L20" s="12"/>
     </row>
     <row r="21" spans="2:12" ht="30" customHeight="1">
       <c r="B21" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>34</v>
@@ -2070,7 +2074,7 @@
       <c r="E21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="14">
         <v>45742</v>
       </c>
       <c r="G21" s="13">
@@ -2080,19 +2084,21 @@
         <f>IF(COUNTA('Controlador de projetos'!$F21,'Controlador de projetos'!$G21)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F21,'Controlador de projetos'!$G21,FALSE))</f>
         <v>2</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="14">
         <v>45742</v>
       </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="15" t="str">
+      <c r="J21" s="13">
+        <v>45744</v>
+      </c>
+      <c r="K21" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I21,'Controlador de projetos'!$J21)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I21,'Controlador de projetos'!$J21,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L21" s="23"/>
+        <v>2</v>
+      </c>
+      <c r="L21" s="12"/>
     </row>
     <row r="22" spans="2:12" ht="30" customHeight="1">
       <c r="B22" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>33</v>
@@ -2103,7 +2109,7 @@
       <c r="E22" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="14">
         <v>45742</v>
       </c>
       <c r="G22" s="13">
@@ -2113,19 +2119,21 @@
         <f>IF(COUNTA('Controlador de projetos'!$F22,'Controlador de projetos'!$G22)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F22,'Controlador de projetos'!$G22,FALSE))</f>
         <v>2</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="14">
         <v>45742</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="15" t="str">
+      <c r="J22" s="13">
+        <v>45744</v>
+      </c>
+      <c r="K22" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I22,'Controlador de projetos'!$J22)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I22,'Controlador de projetos'!$J22,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L22" s="23"/>
+        <v>2</v>
+      </c>
+      <c r="L22" s="12"/>
     </row>
     <row r="23" spans="2:12" ht="42.5" customHeight="1">
       <c r="B23" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>35</v>
@@ -2488,7 +2496,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Ajuste de Títulos de gráficos
</commit_message>
<xml_diff>
--- a/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
+++ b/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C15AE6E-BCA6-4D28-920B-096678F0312B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59696F0B-C7D4-4B13-87C5-623A5DA10A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24620" yWindow="4840" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24480" yWindow="3610" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controlador de projetos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="ColumnTitle1">'Controlador de projetos'!$B$4</definedName>
     <definedName name="ColumnTitle2">Tabela_de_categorias_e_funcionários[[#Headers],[Nome da Categoria]]</definedName>
     <definedName name="Funcionário_Lista">Configuração!$D$5:$D$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$L$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$L$37</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Controlador de projetos'!$4:$4</definedName>
     <definedName name="Sinalizador_Porcentagem">'Controlador de projetos'!#REF!</definedName>
   </definedNames>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="55">
   <si>
     <t>Categoria</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Atualizado em 2025-04-02</t>
+  </si>
+  <si>
+    <t>Revisão de Organização do Documento - Conforme comentário Fase 2</t>
   </si>
 </sst>
 </file>
@@ -1154,8 +1157,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ControladorDeProjetos" displayName="ControladorDeProjetos" ref="B4:L36" totalsRowShown="0" tableBorderDxfId="2">
-  <autoFilter ref="B4:L36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ControladorDeProjetos" displayName="ControladorDeProjetos" ref="B4:L37" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="B4:L37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa" dataCellStyle="Texto"/>
     <tableColumn id="3" xr3:uid="{B833AB72-8646-4CE5-98B8-9D4D27103F03}" name="Responsável" dataCellStyle="Texto"/>
@@ -1430,11 +1433,11 @@
     <tabColor theme="9"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -2189,17 +2192,21 @@
         <f>IF(COUNTA('Controlador de projetos'!$F24,'Controlador de projetos'!$G24)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F24,'Controlador de projetos'!$G24,FALSE)+1)</f>
         <v>26</v>
       </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="15" t="str">
+      <c r="I24" s="14">
+        <v>45777</v>
+      </c>
+      <c r="J24" s="13">
+        <v>45782</v>
+      </c>
+      <c r="K24" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I24,'Controlador de projetos'!$J24)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I24,'Controlador de projetos'!$J24,FALSE)+1)</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="L24" s="12"/>
     </row>
     <row r="25" spans="2:12" ht="30" customHeight="1">
       <c r="B25" s="12" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>36</v>
@@ -2208,7 +2215,7 @@
         <v>19</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F25" s="13">
         <v>45747</v>
@@ -2217,29 +2224,33 @@
         <v>45772</v>
       </c>
       <c r="H25" s="19">
-        <f>IF(COUNTA('Controlador de projetos'!$F25,'Controlador de projetos'!$G25)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F25,'Controlador de projetos'!$G25,FALSE)+1)</f>
-        <v>26</v>
-      </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="15" t="str">
-        <f>IF(COUNTA('Controlador de projetos'!$I25,'Controlador de projetos'!$J25)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I25,'Controlador de projetos'!$J25,FALSE)+1)</f>
-        <v/>
+        <f>IF(COUNTA('Controlador de projetos'!$F25,'Controlador de projetos'!$G25)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F25,'Controlador de projetos'!$G25,FALSE))</f>
+        <v>25</v>
+      </c>
+      <c r="I25" s="14">
+        <v>45772</v>
+      </c>
+      <c r="J25" s="13">
+        <v>45776</v>
+      </c>
+      <c r="K25" s="15">
+        <f>IF(COUNTA('Controlador de projetos'!$I25,'Controlador de projetos'!$J25)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I25,'Controlador de projetos'!$J25,FALSE))</f>
+        <v>4</v>
       </c>
       <c r="L25" s="12"/>
     </row>
     <row r="26" spans="2:12" ht="30" customHeight="1">
       <c r="B26" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F26" s="13">
         <v>45747</v>
@@ -2251,32 +2262,36 @@
         <f>IF(COUNTA('Controlador de projetos'!$F26,'Controlador de projetos'!$G26)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F26,'Controlador de projetos'!$G26,FALSE)+1)</f>
         <v>26</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="15" t="str">
+      <c r="I26" s="14">
+        <v>45772</v>
+      </c>
+      <c r="J26" s="13">
+        <v>45777</v>
+      </c>
+      <c r="K26" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I26,'Controlador de projetos'!$J26)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I26,'Controlador de projetos'!$J26,FALSE)+1)</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="L26" s="12"/>
     </row>
     <row r="27" spans="2:12" ht="30" customHeight="1">
       <c r="B27" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F27" s="13">
-        <v>45775</v>
+        <v>45747</v>
       </c>
       <c r="G27" s="13">
-        <v>45800</v>
+        <v>45772</v>
       </c>
       <c r="H27" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F27,'Controlador de projetos'!$G27)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F27,'Controlador de projetos'!$G27,FALSE)+1)</f>
@@ -2292,7 +2307,7 @@
     </row>
     <row r="28" spans="2:12" ht="30" customHeight="1">
       <c r="B28" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>36</v>
@@ -2301,7 +2316,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F28" s="13">
         <v>45775</v>
@@ -2322,15 +2337,27 @@
       <c r="L28" s="12"/>
     </row>
     <row r="29" spans="2:12" ht="30" customHeight="1">
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="19" t="str">
+      <c r="B29" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="13">
+        <v>45775</v>
+      </c>
+      <c r="G29" s="13">
+        <v>45800</v>
+      </c>
+      <c r="H29" s="19">
         <f>IF(COUNTA('Controlador de projetos'!$F29,'Controlador de projetos'!$G29)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F29,'Controlador de projetos'!$G29,FALSE)+1)</f>
-        <v/>
+        <v>26</v>
       </c>
       <c r="I29" s="14"/>
       <c r="J29" s="13"/>
@@ -2455,33 +2482,52 @@
       <c r="L35" s="12"/>
     </row>
     <row r="36" spans="2:12" ht="30" customHeight="1">
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
       <c r="H36" s="19" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$F36,'Controlador de projetos'!$G36)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F36,'Controlador de projetos'!$G36,FALSE)+1)</f>
         <v/>
       </c>
       <c r="I36" s="14"/>
-      <c r="J36" s="17"/>
+      <c r="J36" s="13"/>
       <c r="K36" s="15" t="str">
         <f>IF(COUNTA('Controlador de projetos'!$I36,'Controlador de projetos'!$J36)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I36,'Controlador de projetos'!$J36,FALSE)+1)</f>
         <v/>
       </c>
-      <c r="L36" s="16"/>
+      <c r="L36" s="12"/>
+    </row>
+    <row r="37" spans="2:12" ht="30" customHeight="1">
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="19" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$F37,'Controlador de projetos'!$G37)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F37,'Controlador de projetos'!$G37,FALSE)+1)</f>
+        <v/>
+      </c>
+      <c r="I37" s="14"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="15" t="str">
+        <f>IF(COUNTA('Controlador de projetos'!$I37,'Controlador de projetos'!$J37)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I37,'Controlador de projetos'!$J37,FALSE)+1)</f>
+        <v/>
+      </c>
+      <c r="L37" s="16"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K5:K36">
+  <conditionalFormatting sqref="K5:K37">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>(ABS((K5-H5))/H5)&gt;Sinalizador_Porcentagem</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" prompt="Insira projetos nesta planilha do controle de projetos. Defina a % acima/abaixo para sinalizar em D2. O trabalho real em horas e a duração real em dias destacarão valores acima/abaixo com negrito, fonte vermelha e um ícone de bandeira nas colunas K e M " sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione uma categoria na lista ou crie uma nova categoria para exibir nesta lista da planilha Configuração." sqref="E5:E36" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione uma categoria na lista ou crie uma nova categoria para exibir nesta lista da planilha Configuração." sqref="E5:E37" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Categoria_Lista</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira os nomes de projetos nesta coluna" sqref="B4:D4" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
@@ -2511,13 +2557,13 @@
           <x14:formula1>
             <xm:f>Configuração!$D$5:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D36</xm:sqref>
+          <xm:sqref>D5:D37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9316C738-7C0B-41CA-ADB5-1A14C6ABE9FF}">
           <x14:formula1>
             <xm:f>Configuração!$C$5:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C36</xm:sqref>
+          <xm:sqref>C5:C37</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Storytelling e formatação final de documentos para entrega.
</commit_message>
<xml_diff>
--- a/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
+++ b/DOCS/Cronograma_Turma_201825166.000.02_Grupo_Projeto_3_V00.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ricardo\Documents\ESTUDO\Mackenzie\02_Sem\PROJ_1\PROJETO\Projeto-Aplicado-1\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59696F0B-C7D4-4B13-87C5-623A5DA10A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8437C366-D009-4014-9C70-6C7F6FBD997A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24480" yWindow="3610" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="4680" windowWidth="24940" windowHeight="22070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controlador de projetos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="ColumnTitle1">'Controlador de projetos'!$B$4</definedName>
     <definedName name="ColumnTitle2">Tabela_de_categorias_e_funcionários[[#Headers],[Nome da Categoria]]</definedName>
     <definedName name="Funcionário_Lista">Configuração!$D$5:$D$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$L$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Controlador de projetos'!$A$1:$K$29</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Controlador de projetos'!$4:$4</definedName>
     <definedName name="Sinalizador_Porcentagem">'Controlador de projetos'!#REF!</definedName>
   </definedNames>
@@ -208,10 +208,10 @@
     <t>Produção de gráficos e tabelas</t>
   </si>
   <si>
-    <t>Atualizado em 2025-04-02</t>
-  </si>
-  <si>
     <t>Revisão de Organização do Documento - Conforme comentário Fase 2</t>
+  </si>
+  <si>
+    <t>Atualizado em 2025-05-05</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1437,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -1463,7 +1463,7 @@
       <c r="A2" s="2"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="3"/>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="25" spans="2:12" ht="30" customHeight="1">
       <c r="B25" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>36</v>
@@ -2297,11 +2297,15 @@
         <f>IF(COUNTA('Controlador de projetos'!$F27,'Controlador de projetos'!$G27)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$F27,'Controlador de projetos'!$G27,FALSE)+1)</f>
         <v>26</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="15" t="str">
+      <c r="I27" s="14">
+        <v>45772</v>
+      </c>
+      <c r="J27" s="13">
+        <v>45782</v>
+      </c>
+      <c r="K27" s="15">
         <f>IF(COUNTA('Controlador de projetos'!$I27,'Controlador de projetos'!$J27)&lt;&gt;2,"",DAYS360('Controlador de projetos'!$I27,'Controlador de projetos'!$J27,FALSE)+1)</f>
-        <v/>
+        <v>11</v>
       </c>
       <c r="L27" s="12"/>
     </row>
@@ -2542,7 +2546,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>